<commit_message>
Adicionado licença e readme.
</commit_message>
<xml_diff>
--- a/Input/Input.xlsx
+++ b/Input/Input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\HW\Kicad\Projs\Teste\Arquivos\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otavi\Documents\Embed\HW\BomPort\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CA580D6-64E3-4316-9DB5-0A4A64BDA657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8D06C99-47FC-4A0B-989C-63AC4F1A83D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>Value</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
+  <si>
+    <t>Company code</t>
   </si>
   <si>
     <t>Description</t>
@@ -58,37 +58,142 @@
     <t>Manufacturer 4</t>
   </si>
   <si>
-    <t>10K</t>
+    <t>RES 1.2K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>R1,R2,R3,R4</t>
+  </si>
+  <si>
+    <t>CRCW08051K20FKEA</t>
+  </si>
+  <si>
+    <t>VISHAY</t>
+  </si>
+  <si>
+    <t>RC0805FR-071K2L</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF1201V</t>
+  </si>
+  <si>
+    <t>PANASONIC</t>
+  </si>
+  <si>
+    <t>RMCF0805FT1K20</t>
+  </si>
+  <si>
+    <t>STACKPOLE</t>
+  </si>
+  <si>
+    <t>RES 3.9K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>R5,R6</t>
+  </si>
+  <si>
+    <t>CRCW08053K90FKEA</t>
+  </si>
+  <si>
+    <t>RC0805FR-073K9L</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF3901V</t>
+  </si>
+  <si>
+    <t>RMCF0805FT3K90</t>
+  </si>
+  <si>
+    <t>RES 6.8K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>CRCW08056K80FKEA</t>
+  </si>
+  <si>
+    <t>RC0805FR-076K8L</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF6801V</t>
+  </si>
+  <si>
+    <t>RMCF0805FT6K80</t>
   </si>
   <si>
     <t>RES 10K OHM 1% 1/8W 0805</t>
   </si>
   <si>
-    <t>R1,R2,R3,R4,R5,R6,R7,R8,R9,R10</t>
+    <t>R8,R9,R10,R11,R12,R13</t>
   </si>
   <si>
     <t>CRCW080510K0FKEA</t>
   </si>
   <si>
-    <t>VISHAY</t>
-  </si>
-  <si>
     <t>RC0805FR-0710KL</t>
   </si>
   <si>
-    <t>YAGEO</t>
-  </si>
-  <si>
-    <t>KTR10EZPF1002</t>
-  </si>
-  <si>
-    <t>ROHM</t>
+    <t>ERJ-6ENF1002V</t>
   </si>
   <si>
     <t>RMCF0805FT10K0</t>
   </si>
   <si>
-    <t>STACKPOLE</t>
+    <t>RES 22K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>R14,R15,R16</t>
+  </si>
+  <si>
+    <t>CRCW080522K0FKEA</t>
+  </si>
+  <si>
+    <t>RC0805FR-0722KL</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF2202V</t>
+  </si>
+  <si>
+    <t>RMCF0805FT22K0</t>
+  </si>
+  <si>
+    <t>RES 47K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>R17,R18,R19,R20,R21,R22,R23,R24</t>
+  </si>
+  <si>
+    <t>CRCW080547K0FKEA</t>
+  </si>
+  <si>
+    <t>RC0805FR-0747KL</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF4702V</t>
+  </si>
+  <si>
+    <t>RMCF0805FT47K0</t>
+  </si>
+  <si>
+    <t>RES 75K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>R25,R26</t>
+  </si>
+  <si>
+    <t>CRCW080575K0FKEA</t>
+  </si>
+  <si>
+    <t>RC0805FR-0775KL</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF7502V</t>
+  </si>
+  <si>
+    <t>RMCF0805FT75K0</t>
   </si>
 </sst>
 </file>
@@ -949,26 +1054,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1009,41 +1099,248 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>20</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" t="s">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>22</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" t="s">
+        <v>51</v>
+      </c>
+      <c r="L7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s">
+        <v>57</v>
+      </c>
+      <c r="L8" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>